<commit_message>
Latest data import scripts + sheets.
</commit_message>
<xml_diff>
--- a/data/Room Legend.xlsx
+++ b/data/Room Legend.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10810"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Macintosh/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Macintosh/github/OpenClassroom/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D307EB7-18C0-1743-82E6-112ACA66CC4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{307F51CB-98F1-884B-8556-77B0CD7D79B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20480" yWindow="0" windowWidth="17920" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15580" yWindow="0" windowWidth="13220" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rooms_SD" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Rooms_SD!$A$31:$B$53</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Rooms_SD!$A$31:$B$49</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="110">
   <si>
     <t>Y-CR1</t>
   </si>
@@ -294,45 +294,24 @@
     <t>UT- Auditorium 3</t>
   </si>
   <si>
-    <t>UTERC-ALR</t>
-  </si>
-  <si>
     <t>ERC - Active Learning Room</t>
   </si>
   <si>
-    <t>UTERC-NAK AUD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ERC - Ngee Ann Kong Si Auditorium </t>
-  </si>
-  <si>
     <t>UTSRC-AUD2</t>
   </si>
   <si>
     <t>SRC - Auditorium 2</t>
   </si>
   <si>
-    <t>UTSRC- GLR</t>
-  </si>
-  <si>
     <t>SRC - Global Learning Room</t>
   </si>
   <si>
-    <t>UTSRC- LT51</t>
-  </si>
-  <si>
     <t>SRC - Lecture Theatre 51</t>
   </si>
   <si>
-    <t>UTSRC- LT52</t>
-  </si>
-  <si>
     <t>SRC - Lecture Theatre 52</t>
   </si>
   <si>
-    <t>UTSRC- LT53</t>
-  </si>
-  <si>
     <t>SRC - Lecture Theatre 53</t>
   </si>
   <si>
@@ -342,19 +321,59 @@
     <t>TP- Auditorium 1</t>
   </si>
   <si>
-    <t>UTTP-GLR</t>
-  </si>
-  <si>
     <t>TP - Global Learning Room</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>ERC-ALR</t>
+  </si>
+  <si>
+    <t>NAK-AUD</t>
+  </si>
+  <si>
+    <t>ERC - Ngee Ann Kong Si Auditorium</t>
+  </si>
+  <si>
+    <t>Y-ELMCL</t>
+  </si>
+  <si>
+    <t>ELM COLLEGE - COMMON LOUNGE</t>
+  </si>
+  <si>
+    <t>Y-YESLab</t>
+  </si>
+  <si>
+    <t>TP-GLR</t>
+  </si>
+  <si>
+    <t>UTSRC-LT53</t>
+  </si>
+  <si>
+    <t>UTSRC-LT51</t>
+  </si>
+  <si>
+    <t>UTSRC-LT52</t>
+  </si>
+  <si>
+    <t>UTSRC-GLR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -381,8 +400,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -663,10 +683,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B54"/>
+  <dimension ref="A1:B56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -998,55 +1018,55 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B41" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B42" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B43" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B44" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>88</v>
+        <v>109</v>
       </c>
       <c r="B45" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>90</v>
+        <v>107</v>
       </c>
       <c r="B46" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="B47" t="s">
         <v>93</v>
@@ -1054,53 +1074,76 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
+        <v>106</v>
+      </c>
+      <c r="B48" t="s">
         <v>94</v>
-      </c>
-      <c r="B48" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
+        <v>95</v>
+      </c>
+      <c r="B49" t="s">
         <v>96</v>
       </c>
-      <c r="B49" t="s">
+    </row>
+    <row r="50" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B56" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>98</v>
-      </c>
-      <c r="B50" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>100</v>
-      </c>
-      <c r="B51" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>102</v>
-      </c>
-      <c r="B52" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>104</v>
-      </c>
-      <c r="B53" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>